<commit_message>
Fix Excel export MergedCell error for template forms
- Add MergedCell check to skip read-only merged cells
- Copy all form templates (1-10) to update_2911 directory
- Add proper exception handling for cell writing
- Fix "Template file not found" error for forms 5-9

Fixes:
- MergedCell object attribute 'value' is read-only error
- Missing template files for forms 1-5, 7-9

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/update_2911/Mẫu 10.xlsx
+++ b/update_2911/Mẫu 10.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CCFB00-9F56-4B9A-BC3D-060183FE71BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Phụ lục 1: DANH SÁCH CỦA CƠ QUAN ĐĂNG KÝ GỬI CÔNG AN CẤP XÃ ĐỂ
 RÀ SOÁT, CẬP NHẬT VÀ BỔ SUNG DỮ LIỆU ĐĂNG KÝ XE; GIẤY PHÉP LÁI XE
@@ -39,6 +38,9 @@
     <t>II. DANH SÁCH XE NỀN MÀU TRẮNG/VÀNG, CHỮ VÀ SỐ MÀU ĐEN</t>
   </si>
   <si>
+    <t>Biển số/ màu biển</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bản sao chứng từ chuyển nhượng (nếu có) </t>
   </si>
   <si>
@@ -57,6 +59,9 @@
     <t>Số CCCD/mã số thuế của chủ xe (tên trong giấy chứng nhận đăng ký xe)</t>
   </si>
   <si>
+    <t>Số GPLX của chủ xe, ngày cấp, cơ quan cấp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tên người bán xe đó và địa chỉ hiện tại của người bán xe </t>
   </si>
   <si>
@@ -64,33 +69,12 @@
   </si>
   <si>
     <t>Số CCCD/mã số thuế người bán xe và người đang sử dụng xe</t>
-  </si>
-  <si>
-    <t>Biển số</t>
-  </si>
-  <si>
-    <t>Màu biển</t>
-  </si>
-  <si>
-    <t>Ngày cấp CCCD/mã số thuế của chủ xe (tên trong giấy chứng nhận đăng ký xe)</t>
-  </si>
-  <si>
-    <t>Số GPLX của chủ xe</t>
-  </si>
-  <si>
-    <t>Ngày cấp GPLX của chủ xe</t>
-  </si>
-  <si>
-    <t>Cơ quan cấp GPLX của chủ xe</t>
-  </si>
-  <si>
-    <t>Ngày cấp CCCD/mã số thuế người bán xe và người đang sử dụng xe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -185,13 +169,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -473,143 +451,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.90625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="9.81640625" style="2" customWidth="1"/>
-    <col min="9" max="11" width="9.90625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.81640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="13" style="2" customWidth="1"/>
-    <col min="14" max="16" width="9.90625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="7.08984375" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="8.90625" style="2"/>
+    <col min="1" max="1" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13" style="2" customWidth="1"/>
+    <col min="10" max="11" width="9.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:17" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" ht="120" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -623,14 +571,9 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -645,13 +588,8 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -666,13 +604,8 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -687,13 +620,8 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -708,13 +636,8 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -729,13 +652,8 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -750,13 +668,8 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -771,13 +684,8 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -792,13 +700,8 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -813,13 +716,8 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -834,36 +732,48 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+    </row>
+    <row r="16" spans="1:12" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -876,15 +786,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -897,15 +802,10 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-    </row>
-    <row r="19" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -918,15 +818,10 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-    </row>
-    <row r="20" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -939,15 +834,10 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-    </row>
-    <row r="21" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -960,15 +850,10 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-    </row>
-    <row r="22" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -981,15 +866,10 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-    </row>
-    <row r="23" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1002,15 +882,10 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-    </row>
-    <row r="24" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1023,15 +898,10 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-    </row>
-    <row r="25" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1044,15 +914,10 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-    </row>
-    <row r="26" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1065,15 +930,10 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-    </row>
-    <row r="27" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1086,15 +946,10 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-    </row>
-    <row r="28" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1107,15 +962,10 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-    </row>
-    <row r="29" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1128,38 +978,44 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-    </row>
-    <row r="30" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
+    </row>
+    <row r="30" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>25</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A31:K31"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix: Restore correct Excel templates and unmerge cells before writing
- Restore Mẫu 6-10 templates from previous update (were overwritten)
- Unmerge cells in data area before writing to prevent format issues
- Remove MergedCell skip logic (now unmerging instead)
- Fix column alignment issues in exported files

Fixes:
- Missing column headers in Mẫu 6 export
- Format errors in certain rows (merged cell conflicts)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/update_2911/Mẫu 10.xlsx
+++ b/update_2911/Mẫu 10.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CCFB00-9F56-4B9A-BC3D-060183FE71BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Phụ lục 1: DANH SÁCH CỦA CƠ QUAN ĐĂNG KÝ GỬI CÔNG AN CẤP XÃ ĐỂ
 RÀ SOÁT, CẬP NHẬT VÀ BỔ SUNG DỮ LIỆU ĐĂNG KÝ XE; GIẤY PHÉP LÁI XE
@@ -38,9 +39,6 @@
     <t>II. DANH SÁCH XE NỀN MÀU TRẮNG/VÀNG, CHỮ VÀ SỐ MÀU ĐEN</t>
   </si>
   <si>
-    <t>Biển số/ màu biển</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bản sao chứng từ chuyển nhượng (nếu có) </t>
   </si>
   <si>
@@ -59,9 +57,6 @@
     <t>Số CCCD/mã số thuế của chủ xe (tên trong giấy chứng nhận đăng ký xe)</t>
   </si>
   <si>
-    <t>Số GPLX của chủ xe, ngày cấp, cơ quan cấp</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tên người bán xe đó và địa chỉ hiện tại của người bán xe </t>
   </si>
   <si>
@@ -69,12 +64,33 @@
   </si>
   <si>
     <t>Số CCCD/mã số thuế người bán xe và người đang sử dụng xe</t>
+  </si>
+  <si>
+    <t>Biển số</t>
+  </si>
+  <si>
+    <t>Màu biển</t>
+  </si>
+  <si>
+    <t>Ngày cấp CCCD/mã số thuế của chủ xe (tên trong giấy chứng nhận đăng ký xe)</t>
+  </si>
+  <si>
+    <t>Số GPLX của chủ xe</t>
+  </si>
+  <si>
+    <t>Ngày cấp GPLX của chủ xe</t>
+  </si>
+  <si>
+    <t>Cơ quan cấp GPLX của chủ xe</t>
+  </si>
+  <si>
+    <t>Ngày cấp CCCD/mã số thuế người bán xe và người đang sử dụng xe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -169,7 +185,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -451,113 +473,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:L16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="11" width="9.88671875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="4.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.90625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="9.81640625" style="2" customWidth="1"/>
+    <col min="9" max="11" width="9.90625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13" style="2" customWidth="1"/>
+    <col min="14" max="16" width="9.90625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="7.08984375" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" ht="120" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -571,9 +623,14 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -588,8 +645,13 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -604,8 +666,13 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -620,8 +687,13 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -636,8 +708,13 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -652,8 +729,13 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -668,8 +750,13 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -684,8 +771,13 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -700,8 +792,13 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -716,8 +813,13 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -732,48 +834,36 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
         <v>12</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
         <v>13</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>12</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -786,10 +876,15 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -802,10 +897,15 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -818,10 +918,15 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -834,10 +939,15 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -850,10 +960,15 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -866,10 +981,15 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -882,10 +1002,15 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -898,10 +1023,15 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -914,10 +1044,15 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -930,10 +1065,15 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -946,10 +1086,15 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -962,10 +1107,15 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -978,44 +1128,38 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
-        <v>25</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="30" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A30:O30"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>